<commit_message>
Atualizando as pastas do repositorio antigo
</commit_message>
<xml_diff>
--- a/Docs/ProductBacklog.xlsx
+++ b/Docs/ProductBacklog.xlsx
@@ -1,16 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aluno\Desktop\projeto-pi\Docs\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="161"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="237"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
     <sheet name="Planilha2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -20,17 +25,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Escopo</t>
   </si>
   <si>
-    <t>Essencial</t>
-  </si>
-  <si>
-    <t>Importante</t>
-  </si>
-  <si>
     <t>Tamanho</t>
   </si>
   <si>
@@ -46,30 +45,15 @@
     <t>ID</t>
   </si>
   <si>
-    <t>Classificação</t>
-  </si>
-  <si>
     <t>O site deverá ter uma tela de login do usuario (Email, senha)</t>
   </si>
   <si>
-    <t>O site deverá ter uma tela de consulta de dados (Temperatura e umidade a cada 30-45 min dependendo do nível de alerta, o quanto a temperatura está alterando)</t>
-  </si>
-  <si>
-    <t>Deverão ter graficos e variação de registros para consultas do cliente (De acordo com os dados coletados no requisito 3)</t>
-  </si>
-  <si>
-    <t>Deverão haver métricas estatisticas para a interpretação dos dados (Interpretação dos dados coletados, para ajudar na tomada de decisão do cliente, por exemplo, níveis de alerta para mudança de temperatura)</t>
-  </si>
-  <si>
     <t>Deverá haver uma aba do nosso site com nosso produto (Contextualização e justificativa do projeto, o que estamos fazendo)</t>
   </si>
   <si>
     <t>Deve haver uma página "Quem somos?" (Quem é o grupo, missão, valores, estratégias ambições, futuro)</t>
   </si>
   <si>
-    <t>Deve haver um logotipo (Clean)</t>
-  </si>
-  <si>
     <t>O site deverá ter uma tela de cadastro do usuario (Nome, Sobrenome, Email, Telefone, CNPJ, senha)</t>
   </si>
   <si>
@@ -79,9 +63,6 @@
     <t>O site deverá conter um simulador financeiro para reforçar os benefícios do produto (Porcentagem de perda por viagem com X produto e quanto economizaria com nossa solução)</t>
   </si>
   <si>
-    <t>Rodar o código no programa do Arduino (O código especificado no requisito 10)</t>
-  </si>
-  <si>
     <t>O sensor de temperatura e umidade deverá ser programado para rodar com o Arduíno (Programação do sensor DHT11 para arduino)</t>
   </si>
   <si>
@@ -94,19 +75,28 @@
     <t>Criar tabelas de banco de dados no Azure (Uma tabela para salvar os dados dos usuários informados no requisito 1 e outra para os dados coletados no arduino)</t>
   </si>
   <si>
-    <t>Os dados coletados pelo sensor deverão ser enviados para o banco de dados no Azure (Conforme requisito 12)</t>
-  </si>
-  <si>
-    <t>Desejável</t>
-  </si>
-  <si>
     <t>TOTAL PONTOS =</t>
+  </si>
+  <si>
+    <t>Deve conter um logotipo (Clean, Relacionado a resfriamento/tecnologia)</t>
+  </si>
+  <si>
+    <t>Ordem Execução</t>
+  </si>
+  <si>
+    <t>Rodar o código no programa do Arduino (O código especificado no requisito 9)</t>
+  </si>
+  <si>
+    <t>Deverá ter uma aba no site contendo os gráficos de variação dos registros (Temperatura e umidade a cada 30-45 min) e métricas estatísticas para interpretar os dados para posterior consulta do cliente (Interpretação dos dados coletados, para ajudar na tomada de decisão do cliente, por exemplo, níveis de alerta para mudança de temperatura)</t>
+  </si>
+  <si>
+    <t>Os dados coletados pelo sensor deverão ser enviados para o banco de dados no Azure (Conforme requisito 11)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -272,7 +262,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -304,9 +294,6 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -324,6 +311,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -596,7 +589,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -604,10 +597,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:J22"/>
+  <dimension ref="B1:J20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -619,16 +612,16 @@
   <sheetData>
     <row r="1" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B1" s="6" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C1" s="6" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E1" s="18" t="s">
-        <v>3</v>
+        <v>18</v>
+      </c>
+      <c r="E1" s="17" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -636,9 +629,9 @@
         <v>1</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="9">
         <v>1</v>
       </c>
       <c r="E2" s="1">
@@ -650,27 +643,27 @@
         <v>2</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="9" t="s">
-        <v>1</v>
+        <v>6</v>
+      </c>
+      <c r="D3" s="9">
+        <v>2</v>
       </c>
       <c r="E3" s="1">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="2:10" ht="29.25" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="7">
         <v>3</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="9" t="s">
-        <v>1</v>
+        <v>17</v>
+      </c>
+      <c r="D4" s="9">
+        <v>3</v>
       </c>
       <c r="E4" s="1">
-        <v>13</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -678,41 +671,41 @@
         <v>4</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" s="9" t="s">
-        <v>1</v>
+        <v>7</v>
+      </c>
+      <c r="D5" s="9">
+        <v>4</v>
       </c>
       <c r="E5" s="1">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="2:10" ht="29.25" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="7">
         <v>5</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" s="9" t="s">
-        <v>1</v>
+        <v>8</v>
+      </c>
+      <c r="D6" s="9">
+        <v>5</v>
       </c>
       <c r="E6" s="1">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B7" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" ht="29.25" x14ac:dyDescent="0.25">
+      <c r="B7" s="22">
         <v>6</v>
       </c>
-      <c r="C7" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" s="9" t="s">
-        <v>2</v>
+      <c r="C7" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="23">
+        <v>6</v>
       </c>
       <c r="E7" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -720,80 +713,80 @@
         <v>7</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D8" s="9" t="s">
-        <v>1</v>
+        <v>10</v>
+      </c>
+      <c r="D8" s="9">
+        <v>7</v>
       </c>
       <c r="E8" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B9" s="7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10" ht="43.5" x14ac:dyDescent="0.25">
+      <c r="B9" s="22">
         <v>8</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="D9" s="9" t="s">
-        <v>25</v>
+        <v>20</v>
+      </c>
+      <c r="D9" s="23">
+        <v>8</v>
       </c>
       <c r="E9" s="1">
-        <v>5</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B10" s="7">
         <v>9</v>
       </c>
-      <c r="C10" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="D10" s="9" t="s">
+      <c r="C10" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="9">
         <v>1</v>
       </c>
-      <c r="E10" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="2:10" ht="29.25" x14ac:dyDescent="0.25">
+      <c r="E10" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B11" s="7">
+        <v>10</v>
+      </c>
+      <c r="C11" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="D11" s="9" t="s">
-        <v>1</v>
+      <c r="D11" s="9">
+        <v>2</v>
       </c>
       <c r="E11" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="J11" s="4"/>
     </row>
     <row r="12" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B12" s="7">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="D12" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="E12" s="11">
-        <v>5</v>
+        <v>13</v>
+      </c>
+      <c r="D12" s="9">
+        <v>3</v>
+      </c>
+      <c r="E12" s="1">
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B13" s="7">
-        <v>11</v>
-      </c>
-      <c r="C13" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="D13" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" s="9">
         <v>1</v>
       </c>
       <c r="E13" s="1">
@@ -802,41 +795,41 @@
     </row>
     <row r="14" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B14" s="7">
-        <v>12</v>
-      </c>
-      <c r="C14" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="D14" s="9">
+        <v>2</v>
+      </c>
+      <c r="E14" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="2:10" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="B15" s="22">
+        <v>14</v>
+      </c>
+      <c r="C15" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="D15" s="9">
+        <v>3</v>
+      </c>
+      <c r="E15" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B16" s="7">
+        <v>15</v>
+      </c>
+      <c r="C16" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="D14" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="E14" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B15" s="7">
-        <v>13</v>
-      </c>
-      <c r="C15" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="D15" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="E15" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="16" spans="2:10" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="B16" s="7">
-        <v>14</v>
-      </c>
-      <c r="C16" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="D16" s="9" t="s">
-        <v>1</v>
+      <c r="D16" s="9">
+        <v>4</v>
       </c>
       <c r="E16" s="1">
         <v>8</v>
@@ -844,79 +837,54 @@
     </row>
     <row r="17" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B17" s="7">
-        <v>15</v>
-      </c>
-      <c r="C17" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="D17" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="E17" s="1">
-        <v>8</v>
+        <v>16</v>
+      </c>
+      <c r="C17" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="D17" s="14">
+        <v>5</v>
+      </c>
+      <c r="E17" s="15">
+        <v>13</v>
       </c>
     </row>
     <row r="18" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B18" s="7">
+        <v>17</v>
+      </c>
+      <c r="C18" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D18" s="9">
+        <v>6</v>
+      </c>
+      <c r="E18" s="18">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B19" s="2"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="20"/>
+    </row>
+    <row r="20" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B20" s="4"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="C18" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="D18" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="E18" s="1">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="19" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B19" s="13">
-        <v>17</v>
-      </c>
-      <c r="C19" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="D19" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="E19" s="16">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="20" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B20" s="7">
-        <v>18</v>
-      </c>
-      <c r="C20" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="D20" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="E20" s="19">
-        <v>3</v>
+      <c r="E20" s="21">
+        <f>SUM(E2:E18)</f>
+        <v>110</v>
       </c>
       <c r="F20" s="4"/>
     </row>
-    <row r="21" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B21" s="2"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="21"/>
-    </row>
-    <row r="22" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B22" s="4"/>
-      <c r="C22" s="4"/>
-      <c r="D22" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="E22" s="22">
-        <f>SUM(E2:E20)</f>
-        <v>144</v>
-      </c>
-    </row>
   </sheetData>
+  <sortState ref="B2:E18">
+    <sortCondition ref="D2"/>
+  </sortState>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>